<commit_message>
Split Ability tab into Ability Cost and Instance
</commit_message>
<xml_diff>
--- a/GameBalanceSheet.xlsx
+++ b/GameBalanceSheet.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Space Attributes" sheetId="3" r:id="rId1"/>
     <sheet name="Character Attributes" sheetId="1" r:id="rId2"/>
     <sheet name="Move Attributes" sheetId="2" r:id="rId3"/>
+    <sheet name="Move Instance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="118">
   <si>
     <t>Character Attributes</t>
   </si>
@@ -326,18 +327,6 @@
   </si>
   <si>
     <t>Extra Instance of Spell Cast (Magical)</t>
-  </si>
-  <si>
-    <t>Damage Over Time</t>
-  </si>
-  <si>
-    <t>Damage Over Next N Turns</t>
-  </si>
-  <si>
-    <t>Damage/Heal Over N Turns</t>
-  </si>
-  <si>
-    <t>Costs (COST)*N*(2/3)</t>
   </si>
   <si>
     <t>Area Independent x1.5</t>
@@ -430,12 +419,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -455,12 +438,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,25 +479,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -574,75 +563,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -988,7 +1006,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
@@ -998,13 +1016,13 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>150</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="28">
         <v>1</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -1012,13 +1030,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="26">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31">
+      <c r="A4" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28">
         <v>1</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -1026,13 +1044,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="26">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31">
+      <c r="A5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1</v>
+      </c>
+      <c r="C5" s="28">
         <v>1</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -1040,13 +1058,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="26">
-        <v>100</v>
-      </c>
-      <c r="C6" s="31">
+      <c r="B6" s="24">
+        <v>100</v>
+      </c>
+      <c r="C6" s="28">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
@@ -1054,13 +1072,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>200</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="28">
         <v>0</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -1068,13 +1086,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="26">
-        <v>100</v>
-      </c>
-      <c r="C8" s="31">
+      <c r="B8" s="24">
+        <v>100</v>
+      </c>
+      <c r="C8" s="28">
         <v>10</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -1082,13 +1100,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>200</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="28">
         <v>1</v>
       </c>
       <c r="D9" s="21" t="s">
@@ -1096,13 +1114,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="26">
-        <v>100</v>
-      </c>
-      <c r="C10" s="31">
+      <c r="B10" s="24">
+        <v>100</v>
+      </c>
+      <c r="C10" s="28">
         <v>25</v>
       </c>
       <c r="D10" s="21" t="s">
@@ -1110,13 +1128,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="26">
-        <v>100</v>
-      </c>
-      <c r="C11" s="31">
+      <c r="B11" s="24">
+        <v>100</v>
+      </c>
+      <c r="C11" s="28">
         <v>10</v>
       </c>
       <c r="D11" s="21" t="s">
@@ -1124,13 +1142,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="26">
-        <v>100</v>
-      </c>
-      <c r="C12" s="31">
+      <c r="B12" s="24">
+        <v>100</v>
+      </c>
+      <c r="C12" s="28">
         <v>10</v>
       </c>
       <c r="D12" s="21" t="s">
@@ -1138,13 +1156,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26">
-        <v>100</v>
-      </c>
-      <c r="C13" s="31">
+      <c r="B13" s="24">
+        <v>100</v>
+      </c>
+      <c r="C13" s="28">
         <v>10</v>
       </c>
       <c r="D13" s="21" t="s">
@@ -1152,45 +1170,45 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="31"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="31"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="31"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="31"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="21"/>
     </row>
   </sheetData>
@@ -1203,8 +1221,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1246,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1255,13 +1273,13 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="A3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25">
         <v>10</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -1270,7 +1288,7 @@
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="27">
         <v>100</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1279,7 +1297,7 @@
       <c r="J3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3" s="27">
         <v>100</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1287,13 +1305,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
-        <v>1</v>
-      </c>
-      <c r="C4" s="27">
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+      <c r="C4" s="25">
         <v>2</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -1302,7 +1320,7 @@
       <c r="F4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="27">
         <v>100</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1311,7 +1329,7 @@
       <c r="J4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="27">
         <v>100</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1319,13 +1337,13 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26">
-        <v>1</v>
-      </c>
-      <c r="C5" s="27">
+      <c r="B5" s="24">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25">
         <v>5</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -1334,7 +1352,7 @@
       <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="27">
         <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1343,7 +1361,7 @@
       <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="27">
         <v>50</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1351,13 +1369,13 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26">
-        <v>1</v>
-      </c>
-      <c r="C6" s="27">
+      <c r="B6" s="24">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
@@ -1366,7 +1384,7 @@
       <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="27">
         <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1375,7 +1393,7 @@
       <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="27">
         <v>20</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1383,97 +1401,97 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>10</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <v>1</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="27">
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="27">
         <v>0</v>
       </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="24">
         <v>10</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="25">
         <v>1</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="27">
         <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="27">
         <v>0</v>
       </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>10</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <v>1</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="27">
         <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="27">
         <v>0</v>
       </c>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="26">
-        <v>1</v>
-      </c>
-      <c r="C10" s="27">
+      <c r="B10" s="24">
+        <v>1</v>
+      </c>
+      <c r="C10" s="25">
         <v>5</v>
       </c>
       <c r="D10" s="21" t="s">
@@ -1482,7 +1500,7 @@
       <c r="F10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="27">
         <v>100</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1491,7 +1509,7 @@
       <c r="J10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="27">
         <v>100</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1499,13 +1517,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="26">
-        <v>100</v>
-      </c>
-      <c r="C11" s="27">
+      <c r="B11" s="24">
+        <v>100</v>
+      </c>
+      <c r="C11" s="25">
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
@@ -1514,7 +1532,7 @@
       <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="27">
         <v>100</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1523,7 +1541,7 @@
       <c r="J11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="27">
         <v>100</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1531,91 +1549,91 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="26">
+      <c r="A12" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="24">
         <v>25</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>1</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="30"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="1"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="30"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="26">
+      <c r="A13" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="24">
         <v>25</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <v>2</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="30"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="1"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="30"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="24">
+        <v>50</v>
+      </c>
+      <c r="C14" s="25">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="26">
-        <v>50</v>
-      </c>
-      <c r="C14" s="27">
-        <v>1</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>120</v>
-      </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="30"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="1"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="30"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="26">
-        <v>100</v>
-      </c>
-      <c r="C15" s="27">
+      <c r="B15" s="24">
+        <v>100</v>
+      </c>
+      <c r="C15" s="25">
         <v>1</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="27">
         <v>400</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="27">
         <v>400</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1623,13 +1641,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="26">
-        <v>100</v>
-      </c>
-      <c r="C16" s="27">
+      <c r="B16" s="24">
+        <v>100</v>
+      </c>
+      <c r="C16" s="25">
         <v>25</v>
       </c>
       <c r="D16" s="21" t="s">
@@ -1638,7 +1656,7 @@
       <c r="F16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="27">
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -1647,7 +1665,7 @@
       <c r="J16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="27">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -1655,13 +1673,13 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="26">
-        <v>100</v>
-      </c>
-      <c r="C17" s="27">
+      <c r="B17" s="24">
+        <v>100</v>
+      </c>
+      <c r="C17" s="25">
         <v>25</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -1670,7 +1688,7 @@
       <c r="F17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="27">
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -1679,7 +1697,7 @@
       <c r="J17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="27">
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1687,22 +1705,22 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="26">
-        <v>100</v>
-      </c>
-      <c r="C18" s="27">
+      <c r="B18" s="24">
+        <v>100</v>
+      </c>
+      <c r="C18" s="25">
         <v>25</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="27">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -1711,7 +1729,7 @@
       <c r="J18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="27">
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -1719,22 +1737,22 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="26">
-        <v>100</v>
-      </c>
-      <c r="C19" s="27">
+      <c r="B19" s="24">
+        <v>100</v>
+      </c>
+      <c r="C19" s="25">
         <v>25</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="27">
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -1743,7 +1761,7 @@
       <c r="J19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="27">
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -1751,13 +1769,13 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="26">
-        <v>100</v>
-      </c>
-      <c r="C20" s="27">
+      <c r="B20" s="24">
+        <v>100</v>
+      </c>
+      <c r="C20" s="25">
         <v>10</v>
       </c>
       <c r="D20" s="21" t="s">
@@ -1766,7 +1784,7 @@
       <c r="F20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="27">
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1775,7 +1793,7 @@
       <c r="J20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="27">
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -1783,13 +1801,13 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="26">
-        <v>100</v>
-      </c>
-      <c r="C21" s="27">
+      <c r="B21" s="24">
+        <v>100</v>
+      </c>
+      <c r="C21" s="25">
         <v>10</v>
       </c>
       <c r="D21" s="21" t="s">
@@ -1798,7 +1816,7 @@
       <c r="F21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="27">
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1807,7 +1825,7 @@
       <c r="J21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="27">
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -1815,13 +1833,13 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="24">
         <v>200</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="25">
         <v>15</v>
       </c>
       <c r="D22" s="21" t="s">
@@ -1830,7 +1848,7 @@
       <c r="F22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="27">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -1839,7 +1857,7 @@
       <c r="J22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="30">
+      <c r="K22" s="27">
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -2062,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>7</v>
@@ -2238,60 +2256,54 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="31"/>
     <col min="4" max="4" width="55.140625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="66" customWidth="1"/>
     <col min="8" max="8" width="33.7109375" customWidth="1"/>
-    <col min="10" max="10" width="46.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="11" max="11" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="4">
-        <f>SUM(I$3:I$31)</f>
-        <v>450</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28">
         <v>1</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -2299,24 +2311,15 @@
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
-      <c r="H3" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="33">
-        <v>100</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>25</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="28">
         <v>1</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -2324,24 +2327,15 @@
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="21"/>
-      <c r="H4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="33">
-        <v>100</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="26">
-        <v>50</v>
-      </c>
-      <c r="C5" s="27">
+      <c r="B5" s="24">
+        <v>50</v>
+      </c>
+      <c r="C5" s="28">
         <v>1</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -2351,18 +2345,15 @@
       <c r="F5" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="24">
         <v>25</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="28">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
@@ -2372,18 +2363,15 @@
       <c r="F6" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="26">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="24">
         <v>75</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="28">
         <v>1</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -2393,18 +2381,15 @@
       <c r="F7" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="32"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="26">
-        <v>1</v>
-      </c>
-      <c r="C8" s="27">
+      <c r="B8" s="24">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28">
         <v>1</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2414,24 +2399,15 @@
       <c r="F8" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H8" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="33">
-        <v>0</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>75</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="28">
         <v>1</v>
       </c>
       <c r="D9" s="21" t="s">
@@ -2441,24 +2417,15 @@
       <c r="F9" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="33">
-        <v>0</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="24">
         <v>25</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="28">
         <v>1</v>
       </c>
       <c r="D10" s="21" t="s">
@@ -2470,24 +2437,15 @@
       <c r="F10" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="33">
-        <v>0</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="24">
         <v>25</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="28">
         <v>2</v>
       </c>
       <c r="D11" s="21" t="s">
@@ -2499,18 +2457,15 @@
       <c r="F11" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="32"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="26">
-        <v>50</v>
-      </c>
-      <c r="C12" s="27">
+      <c r="B12" s="24">
+        <v>50</v>
+      </c>
+      <c r="C12" s="28">
         <v>1</v>
       </c>
       <c r="D12" s="21" t="s">
@@ -2518,18 +2473,15 @@
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="26">
-        <v>100</v>
-      </c>
-      <c r="C13" s="27">
+      <c r="B13" s="24">
+        <v>100</v>
+      </c>
+      <c r="C13" s="28">
         <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
@@ -2537,18 +2489,15 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="21"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="32"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="26">
-        <v>1</v>
-      </c>
-      <c r="C14" s="27">
+      <c r="B14" s="24">
+        <v>1</v>
+      </c>
+      <c r="C14" s="28">
         <v>1</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -2556,24 +2505,15 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="21"/>
-      <c r="H14" s="32" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="24">
         <v>25</v>
       </c>
-      <c r="I14" s="33">
-        <v>0</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="26">
-        <v>25</v>
-      </c>
-      <c r="C15" s="27">
+      <c r="C15" s="28">
         <v>1</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -2581,24 +2521,15 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="21"/>
-      <c r="H15" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="33">
-        <v>0</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="24">
         <v>75</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="28">
         <v>1</v>
       </c>
       <c r="D16" s="21" t="s">
@@ -2606,24 +2537,15 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
-      <c r="H16" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="33">
-        <v>100</v>
-      </c>
-      <c r="J16" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="24">
         <v>75</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="28">
         <v>2</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2631,18 +2553,15 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="21"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="24">
         <v>150</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="28">
         <v>1</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -2650,18 +2569,15 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="32"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="26">
-        <v>100</v>
-      </c>
-      <c r="C19" s="27">
+      <c r="B19" s="24">
+        <v>100</v>
+      </c>
+      <c r="C19" s="28">
         <v>1</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -2669,18 +2585,15 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="21"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="26">
-        <v>100</v>
-      </c>
-      <c r="C20" s="27">
+      <c r="B20" s="24">
+        <v>100</v>
+      </c>
+      <c r="C20" s="28">
         <v>10</v>
       </c>
       <c r="D20" s="21" t="s">
@@ -2688,24 +2601,15 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="21"/>
-      <c r="H20" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="33">
-        <v>100</v>
-      </c>
-      <c r="J20" s="32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="26">
-        <v>100</v>
-      </c>
-      <c r="C21" s="27">
+      <c r="B21" s="24">
+        <v>100</v>
+      </c>
+      <c r="C21" s="28">
         <v>50</v>
       </c>
       <c r="D21" s="21" t="s">
@@ -2713,566 +2617,783 @@
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="21"/>
-      <c r="H21" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="33">
-        <v>50</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="26">
-        <v>10</v>
-      </c>
-      <c r="C22" s="27">
-        <v>15</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>101</v>
-      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="21"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33">
-        <v>0</v>
-      </c>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="21"/>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="24">
+        <v>100</v>
+      </c>
+      <c r="C24" s="28">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>44</v>
+      </c>
       <c r="E24" s="20"/>
       <c r="F24" s="21"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="33">
-        <v>0</v>
-      </c>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="26">
-        <v>100</v>
-      </c>
-      <c r="C25" s="27">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="24">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28">
         <v>1</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="21"/>
-      <c r="H25" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" s="33">
-        <v>0</v>
-      </c>
-      <c r="J25" s="32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="31">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="24">
+        <v>1</v>
+      </c>
+      <c r="C26" s="28">
         <v>1</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
-      <c r="H26" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="33">
-        <v>0</v>
-      </c>
-      <c r="J26" s="32"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="26">
-        <v>1</v>
-      </c>
-      <c r="C27" s="31">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="24">
+        <v>100</v>
+      </c>
+      <c r="C27" s="28">
         <v>1</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="21"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="32"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="26">
-        <v>100</v>
-      </c>
-      <c r="C28" s="31">
-        <v>1</v>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="24">
+        <v>200</v>
+      </c>
+      <c r="C28" s="28">
+        <v>0</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="21"/>
-      <c r="H28" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" s="33">
-        <v>0</v>
-      </c>
-      <c r="J28" s="32"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="26">
-        <v>200</v>
-      </c>
-      <c r="C29" s="31">
-        <v>0</v>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="24">
+        <v>100</v>
+      </c>
+      <c r="C29" s="28">
+        <v>1</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="21"/>
-      <c r="H29" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="33">
-        <v>0</v>
-      </c>
-      <c r="J29" s="32"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="26">
-        <v>100</v>
-      </c>
-      <c r="C30" s="27">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="24">
+        <v>100</v>
+      </c>
+      <c r="C30" s="28">
         <v>1</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="21"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="32"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="26">
-        <v>100</v>
-      </c>
-      <c r="C31" s="27">
-        <v>1</v>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="24">
+        <v>100</v>
+      </c>
+      <c r="C31" s="28">
+        <v>15</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="21"/>
-      <c r="H31" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="33">
-        <v>0</v>
-      </c>
-      <c r="J31" s="32"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="26">
-        <v>100</v>
-      </c>
-      <c r="C32" s="27">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
+      <c r="B32" s="24">
+        <v>100</v>
+      </c>
+      <c r="C32" s="28">
+        <v>15</v>
+      </c>
       <c r="D32" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="21"/>
-      <c r="H32" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="33">
-        <v>1</v>
-      </c>
-      <c r="J32" s="32"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="24">
+        <v>100</v>
+      </c>
+      <c r="C33" s="28">
         <v>15</v>
       </c>
-      <c r="B33" s="26">
-        <v>100</v>
-      </c>
-      <c r="C33" s="27">
-        <v>15</v>
-      </c>
       <c r="D33" s="21" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="21"/>
-      <c r="H33" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="I33" s="33">
-        <v>2</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="26">
-        <v>100</v>
-      </c>
-      <c r="C34" s="27">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="24">
+        <v>100</v>
+      </c>
+      <c r="C34" s="28">
         <v>15</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="21"/>
-      <c r="H34" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" s="33">
-        <v>3</v>
-      </c>
-      <c r="J34" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="26">
-        <v>100</v>
-      </c>
-      <c r="C35" s="27">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="24">
+        <v>100</v>
+      </c>
+      <c r="C35" s="28">
         <v>15</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="26">
-        <v>100</v>
-      </c>
-      <c r="C36" s="27">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="24">
+        <v>100</v>
+      </c>
+      <c r="C36" s="28">
         <v>15</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="21"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="26">
-        <v>100</v>
-      </c>
-      <c r="C37" s="27">
-        <v>15</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="24">
+        <v>100</v>
+      </c>
+      <c r="C37" s="28">
+        <v>50</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="21"/>
-      <c r="H37" s="24" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4">
+        <f>SUM(B$3:B$30)</f>
+        <v>1300</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="I37" s="35">
-        <f>I3*$C3/$B3</f>
-        <v>100</v>
-      </c>
-      <c r="J37" s="24" t="s">
+      <c r="B2" s="30">
+        <v>50</v>
+      </c>
+      <c r="C2" s="36">
+        <f>'Move Instance'!B2*'Move Attributes'!C3/'Move Attributes'!B3</f>
+        <v>50</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="30">
+        <v>50</v>
+      </c>
+      <c r="C3" s="36">
+        <f>'Move Instance'!B3*'Move Attributes'!C4/'Move Attributes'!B4</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="30">
+        <v>50</v>
+      </c>
+      <c r="C4" s="36">
+        <f>'Move Instance'!B4*'Move Attributes'!C5/'Move Attributes'!B5</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="30">
+        <v>50</v>
+      </c>
+      <c r="C5" s="36">
+        <f>'Move Instance'!B5*'Move Attributes'!C6/'Move Attributes'!B6</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="30">
+        <v>50</v>
+      </c>
+      <c r="C6" s="36">
+        <f>'Move Instance'!B6*'Move Attributes'!C7/'Move Attributes'!B7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="30">
+        <v>50</v>
+      </c>
+      <c r="C7" s="38">
+        <f>'Move Instance'!B7*'Move Attributes'!C8/'Move Attributes'!B8</f>
+        <v>50</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="30">
+        <v>50</v>
+      </c>
+      <c r="C8" s="38">
+        <f>'Move Instance'!B8*'Move Attributes'!C9/'Move Attributes'!B9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="30">
+        <v>50</v>
+      </c>
+      <c r="C9" s="38">
+        <f>'Move Instance'!B9*'Move Attributes'!C10/'Move Attributes'!B10</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="30">
+        <v>50</v>
+      </c>
+      <c r="C10" s="38">
+        <f>'Move Instance'!B10*'Move Attributes'!C11/'Move Attributes'!B11</f>
+        <v>4</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="30">
+        <v>50</v>
+      </c>
+      <c r="C11" s="38">
+        <f>'Move Instance'!B11*'Move Attributes'!C12/'Move Attributes'!B12</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="30">
+        <v>50</v>
+      </c>
+      <c r="C12" s="38">
+        <f>'Move Instance'!B12*'Move Attributes'!C13/'Move Attributes'!B13</f>
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="30">
+        <v>50</v>
+      </c>
+      <c r="C13" s="40">
+        <f>'Move Instance'!B13*'Move Attributes'!C14/'Move Attributes'!B14</f>
+        <v>50</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="30">
+        <v>50</v>
+      </c>
+      <c r="C14" s="40">
+        <f>'Move Instance'!B14*'Move Attributes'!C15/'Move Attributes'!B15</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="30">
+        <v>50</v>
+      </c>
+      <c r="C15" s="40">
+        <f>'Move Instance'!B15*'Move Attributes'!C16/'Move Attributes'!B16</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="30">
+        <v>50</v>
+      </c>
+      <c r="C16" s="40">
+        <f>'Move Instance'!B16*'Move Attributes'!C17/'Move Attributes'!B17</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="30">
+        <v>50</v>
+      </c>
+      <c r="C17" s="40">
+        <f>'Move Instance'!B17*'Move Attributes'!C18/'Move Attributes'!B18</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="30">
+        <v>50</v>
+      </c>
+      <c r="C18" s="40">
+        <f>'Move Instance'!B18*'Move Attributes'!C19/'Move Attributes'!B19</f>
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="30">
+        <v>50</v>
+      </c>
+      <c r="C19" s="43">
+        <f>'Move Instance'!B19*'Move Attributes'!C20/'Move Attributes'!B20</f>
+        <v>5</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="26">
-        <v>100</v>
-      </c>
-      <c r="C38" s="27">
-        <v>50</v>
-      </c>
-      <c r="D38" s="21" t="s">
+      <c r="B20" s="30">
+        <v>50</v>
+      </c>
+      <c r="C20" s="43">
+        <f>'Move Instance'!B20*'Move Attributes'!C21/'Move Attributes'!B21</f>
+        <v>25</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="H38" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="35">
-        <f>I4*$C4/$B4</f>
-        <v>4</v>
-      </c>
-      <c r="J38" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H39" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="6">
-        <f>I8*$C8/$B8</f>
-        <v>0</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H40" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="6">
-        <f>I9*$C9/$B9</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="6">
-        <f>I10*$C10/$B10</f>
-        <v>0</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H42" s="25" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="29"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="45">
+        <v>50</v>
+      </c>
+      <c r="C23" s="46">
+        <f>'Move Instance'!B23*'Move Attributes'!C24/'Move Attributes'!B24</f>
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="48">
+        <v>50</v>
+      </c>
+      <c r="C24" s="36">
+        <f>'Move Instance'!B24*'Move Attributes'!C25/'Move Attributes'!B25</f>
+        <v>50</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="49">
+        <v>50</v>
+      </c>
+      <c r="C25" s="40">
+        <f>'Move Instance'!B25*'Move Attributes'!C26/'Move Attributes'!B26</f>
+        <v>50</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="22">
+        <v>50</v>
+      </c>
+      <c r="C26" s="47">
+        <f>'Move Instance'!B26*'Move Attributes'!C27/'Move Attributes'!B27</f>
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="51">
+        <v>50</v>
+      </c>
+      <c r="C27" s="42">
+        <f>'Move Instance'!B27*'Move Attributes'!C28/'Move Attributes'!B28</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="50">
+        <v>50</v>
+      </c>
+      <c r="C28" s="38">
+        <f>'Move Instance'!B28*'Move Attributes'!C29/'Move Attributes'!B29</f>
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="50">
+        <v>50</v>
+      </c>
+      <c r="C29" s="38">
+        <f>'Move Instance'!B29*'Move Attributes'!C30/'Move Attributes'!B30</f>
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="50">
+        <v>50</v>
+      </c>
+      <c r="C30" s="38">
+        <f>'Move Instance'!B30*'Move Attributes'!C31/'Move Attributes'!B31</f>
+        <v>7.5</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="50">
+        <v>50</v>
+      </c>
+      <c r="C31" s="38">
+        <f>'Move Instance'!B31*'Move Attributes'!C32/'Move Attributes'!B32</f>
+        <v>7.5</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I42" s="34">
-        <f>I14*$C14/$B14</f>
-        <v>0</v>
-      </c>
-      <c r="J42" s="25" t="s">
+      <c r="B32" s="49">
+        <v>50</v>
+      </c>
+      <c r="C32" s="40">
+        <f>'Move Instance'!B32*'Move Attributes'!C33/'Move Attributes'!B33</f>
+        <v>7.5</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="49">
+        <v>50</v>
+      </c>
+      <c r="C33" s="40">
+        <f>'Move Instance'!B33*'Move Attributes'!C34/'Move Attributes'!B34</f>
+        <v>7.5</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="50">
+        <v>50</v>
+      </c>
+      <c r="C34" s="38">
+        <f>'Move Instance'!B34*'Move Attributes'!C35/'Move Attributes'!B35</f>
+        <v>7.5</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="50">
+        <v>50</v>
+      </c>
+      <c r="C35" s="38">
+        <f>'Move Instance'!B35*'Move Attributes'!C36/'Move Attributes'!B36</f>
+        <v>7.5</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="48">
+        <v>50</v>
+      </c>
+      <c r="C36" s="36">
+        <f>'Move Instance'!B36*'Move Attributes'!C37/'Move Attributes'!B37</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H43" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I43" s="34">
-        <f>I15*$C15/$B15</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H44" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" s="34">
-        <f>I16*$C16/$B16</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J44" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H45" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="6">
-        <f>I20*$C20/$B20</f>
-        <v>10</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H46" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="37">
-        <f>I21*$C21/$B21</f>
-        <v>25</v>
-      </c>
-      <c r="J46" s="36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H47" s="32"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="32"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H48" s="32"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="32"/>
-    </row>
-    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H49" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="I49" s="39">
-        <f>I25*$C25/$B25</f>
-        <v>0</v>
-      </c>
-      <c r="J49" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H50" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I50" s="6">
-        <f>I26*$C30/$B30</f>
-        <v>0</v>
-      </c>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I51" s="6">
-        <f>I28*$C32/$B32</f>
-        <v>0</v>
-      </c>
-      <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H52" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" s="38">
-        <f>I29*$C33/$B33</f>
-        <v>0</v>
-      </c>
-      <c r="J52" s="28"/>
-    </row>
-    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H53" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" s="22">
-        <f>I31*$C35/$B35</f>
-        <v>0</v>
-      </c>
-      <c r="J53" s="23"/>
-    </row>
-    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H54" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I54" s="35">
-        <f>I32*$C36/$B36</f>
-        <v>0.15</v>
-      </c>
-      <c r="J54" s="24"/>
-    </row>
-    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H55" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I55" s="6">
-        <f>I33*$C37/$B37</f>
-        <v>0.3</v>
-      </c>
-      <c r="J55" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H56" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="I56" s="37">
-        <f>I34*$C38/$B38</f>
-        <v>1.5</v>
-      </c>
-      <c r="J56" s="36" t="s">
+      <c r="D36" s="35" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>